<commit_message>
Saving OPTICS excel file after changing selected blue
</commit_message>
<xml_diff>
--- a/OPTICS predictions t1 aa model .xlsx
+++ b/OPTICS predictions t1 aa model .xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oakley/Documents/GitHub/cyano_rhodopsins/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DDA23CA-B752-C747-A1FD-887839E78EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74849ECF-A0AA-0246-AA38-9DBBBC3A58CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="760" windowWidth="15740" windowHeight="20400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1640" yWindow="760" windowWidth="21020" windowHeight="20280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -18,15 +18,13 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Sheet!$B$1</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Sheet!$B$2:$B$830</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet!$B$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet!$B$2:$B$830</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2492" uniqueCount="1026">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2493" uniqueCount="1027">
   <si>
     <t>Names</t>
   </si>
@@ -3104,13 +3102,16 @@
   </si>
   <si>
     <t>f02</t>
+  </si>
+  <si>
+    <t>No Lysine -- removed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3119,6 +3120,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -4292,7 +4301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="193">
+  <cellXfs count="194">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -4486,6 +4495,7 @@
     <xf numFmtId="0" fontId="0" fillId="191" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="192" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5486,10 +5496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E830"/>
+  <dimension ref="A1:G830"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A795" workbookViewId="0">
+      <selection activeCell="A821" sqref="A821"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19369,7 +19379,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="817" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="817" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A817" t="s">
         <v>411</v>
       </c>
@@ -19386,7 +19396,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="818" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="818" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A818" t="s">
         <v>457</v>
       </c>
@@ -19403,7 +19413,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="819" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="819" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A819" t="s">
         <v>967</v>
       </c>
@@ -19420,8 +19430,8 @@
         <v>412</v>
       </c>
     </row>
-    <row r="820" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A820" s="192" t="s">
+    <row r="820" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A820" s="193" t="s">
         <v>977</v>
       </c>
       <c r="B820">
@@ -19436,8 +19446,11 @@
       <c r="E820" s="187" t="s">
         <v>978</v>
       </c>
-    </row>
-    <row r="821" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G820" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="821" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A821" t="s">
         <v>435</v>
       </c>
@@ -19454,7 +19467,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="822" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="822" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A822" t="s">
         <v>920</v>
       </c>
@@ -19471,7 +19484,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="823" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="823" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A823" s="192" t="s">
         <v>997</v>
       </c>
@@ -19488,7 +19501,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="824" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="824" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A824" t="s">
         <v>290</v>
       </c>
@@ -19505,7 +19518,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="825" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="825" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A825" t="s">
         <v>853</v>
       </c>
@@ -19522,7 +19535,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="826" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="826" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A826" s="192" t="s">
         <v>928</v>
       </c>
@@ -19539,7 +19552,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="827" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="827" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A827" t="s">
         <v>263</v>
       </c>
@@ -19556,7 +19569,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="828" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="828" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A828" t="s">
         <v>273</v>
       </c>
@@ -19573,7 +19586,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="829" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="829" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A829" t="s">
         <v>834</v>
       </c>
@@ -19590,7 +19603,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="830" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="830" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A830" s="192" t="s">
         <v>909</v>
       </c>

</xml_diff>